<commit_message>
careers now have randomly set paths, sims can get promoted
</commit_message>
<xml_diff>
--- a/career_info.xlsx
+++ b/career_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Path</t>
   </si>
@@ -46,9 +46,21 @@
     <t>Expenses Assistant</t>
   </si>
   <si>
+    <t>Payments Assistant</t>
+  </si>
+  <si>
+    <t>Accounts Receivable Assistant</t>
+  </si>
+  <si>
     <t>Accounts Payable Assistant</t>
   </si>
   <si>
+    <t>Senior Accounts Payable Assistant</t>
+  </si>
+  <si>
+    <t>Senior Accounts Receivable Assistant</t>
+  </si>
+  <si>
     <t>Accounts Assistant</t>
   </si>
   <si>
@@ -70,6 +82,9 @@
     <t>CEO</t>
   </si>
   <si>
+    <t>Monday, Tuesday, Wednesday, Thursday</t>
+  </si>
+  <si>
     <t>Culinary</t>
   </si>
   <si>
@@ -80,6 +95,18 @@
   </si>
   <si>
     <t>Salad Prep</t>
+  </si>
+  <si>
+    <t>Line Cook</t>
+  </si>
+  <si>
+    <t>Dessert Specialist</t>
+  </si>
+  <si>
+    <t>Sous Chef</t>
+  </si>
+  <si>
+    <t>Head Chef</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1310,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -1292,7 +1319,7 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.9219" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
     <col min="5" max="6" width="40.0547" style="1" customWidth="1"/>
     <col min="7" max="256" width="16.3516" style="1" customWidth="1"/>
@@ -1332,7 +1359,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="4">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s" s="3">
         <v>8</v>
@@ -1383,7 +1410,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s" s="5">
         <v>11</v>
@@ -1403,13 +1430,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s" s="5">
         <v>12</v>
       </c>
       <c r="D6" s="6">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6">
         <v>7.5</v>
@@ -1423,13 +1450,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s" s="5">
         <v>13</v>
       </c>
       <c r="D7" s="6">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6">
         <v>7.5</v>
@@ -1438,41 +1465,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
+    <row r="8" ht="32.05" customHeight="1">
       <c r="A8" t="s" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s" s="5">
         <v>14</v>
       </c>
       <c r="D8" s="6">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E8" s="6">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="F8" t="s" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
+    <row r="9" ht="32.05" customHeight="1">
       <c r="A9" t="s" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s" s="5">
         <v>15</v>
       </c>
       <c r="D9" s="6">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="E9" s="6">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="F9" t="s" s="5">
         <v>8</v>
@@ -1483,16 +1510,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s" s="5">
         <v>16</v>
       </c>
       <c r="D10" s="6">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="E10" s="6">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="F10" t="s" s="5">
         <v>8</v>
@@ -1503,16 +1530,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s" s="5">
         <v>17</v>
       </c>
       <c r="D11" s="6">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="F11" t="s" s="5">
         <v>8</v>
@@ -1523,16 +1550,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s" s="5">
         <v>18</v>
       </c>
       <c r="D12" s="6">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="E12" s="6">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s" s="5">
         <v>8</v>
@@ -1540,42 +1567,202 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="5">
-        <v>20</v>
-      </c>
       <c r="D13" s="6">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="E13" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="5">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B14" s="6">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6">
+        <v>80</v>
+      </c>
+      <c r="E14" s="6">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6">
+        <v>95</v>
+      </c>
+      <c r="E15" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="F15" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D16" s="6">
+        <v>110</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="F16" t="s" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="D17" s="6">
+        <v>9</v>
+      </c>
+      <c r="E17" s="6">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C14" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="C18" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="D18" s="6">
         <v>12</v>
       </c>
-      <c r="E14" s="6">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s" s="5">
-        <v>21</v>
+      <c r="E18" s="6">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D19" s="6">
+        <v>15</v>
+      </c>
+      <c r="E19" s="6">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B20" s="6">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="D20" s="6">
+        <v>18</v>
+      </c>
+      <c r="E20" s="6">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B21" s="6">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6">
+        <v>28</v>
+      </c>
+      <c r="E21" s="6">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B22" s="6">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="D22" s="6">
+        <v>40</v>
+      </c>
+      <c r="E22" s="6">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s" s="5">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new career path added
</commit_message>
<xml_diff>
--- a/career_info.xlsx
+++ b/career_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>Path</t>
   </si>
@@ -107,6 +107,54 @@
   </si>
   <si>
     <t>Head Chef</t>
+  </si>
+  <si>
+    <t>Restauranteur</t>
+  </si>
+  <si>
+    <t>Franchise Owner</t>
+  </si>
+  <si>
+    <t>Celebrity Chef</t>
+  </si>
+  <si>
+    <t>Tuesday, Friday, Saturday, Sunday</t>
+  </si>
+  <si>
+    <t>Culinary Legend</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Legal Assistant</t>
+  </si>
+  <si>
+    <t>Cost Draftsperson</t>
+  </si>
+  <si>
+    <t>Paralegal</t>
+  </si>
+  <si>
+    <t>Trainee Lawyer</t>
+  </si>
+  <si>
+    <t>Junior Associate</t>
+  </si>
+  <si>
+    <t>Associate</t>
+  </si>
+  <si>
+    <t>Senior Associate</t>
+  </si>
+  <si>
+    <t>Legal Director</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Senior Parter</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1358,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -1319,9 +1367,10 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="6" width="40.0547" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.35156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.0547" style="1" customWidth="1"/>
     <col min="7" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1465,7 +1514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="32.05" customHeight="1">
+    <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="5">
         <v>6</v>
       </c>
@@ -1485,7 +1534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" ht="32.05" customHeight="1">
+    <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="5">
         <v>6</v>
       </c>
@@ -1636,7 +1685,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="6">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="E16" s="6">
         <v>6.5</v>
@@ -1763,6 +1812,286 @@
       </c>
       <c r="F22" t="s" s="5">
         <v>26</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="D23" s="6">
+        <v>55</v>
+      </c>
+      <c r="E23" s="6">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B24" s="6">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="D24" s="6">
+        <v>75</v>
+      </c>
+      <c r="E24" s="6">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="D25" s="6">
+        <v>100</v>
+      </c>
+      <c r="E25" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="F25" t="s" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="D26" s="6">
+        <v>100</v>
+      </c>
+      <c r="E26" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="F26" t="s" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="D27" s="6">
+        <v>10</v>
+      </c>
+      <c r="E27" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F27" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="D28" s="6">
+        <v>15</v>
+      </c>
+      <c r="E28" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F28" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B29" s="6">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="D29" s="6">
+        <v>20</v>
+      </c>
+      <c r="E29" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F29" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B30" s="6">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="D30" s="6">
+        <v>35</v>
+      </c>
+      <c r="E30" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F30" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B31" s="6">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s" s="5">
+        <v>42</v>
+      </c>
+      <c r="D31" s="6">
+        <v>55</v>
+      </c>
+      <c r="E31" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F31" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B32" s="6">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="D32" s="6">
+        <v>70</v>
+      </c>
+      <c r="E32" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F32" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B33" s="6">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="D33" s="6">
+        <v>85</v>
+      </c>
+      <c r="E33" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="F33" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B34" s="6">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="D34" s="6">
+        <v>95</v>
+      </c>
+      <c r="E34" s="6">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B35" s="6">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s" s="5">
+        <v>46</v>
+      </c>
+      <c r="D35" s="6">
+        <v>110</v>
+      </c>
+      <c r="E35" s="6">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="B36" s="6">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s" s="5">
+        <v>47</v>
+      </c>
+      <c r="D36" s="6">
+        <v>125</v>
+      </c>
+      <c r="E36" s="6">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>